<commit_message>
added AY_Prototype csv with sample random data in correct format, added veilofignorance.ipynb for mongodb script
</commit_message>
<xml_diff>
--- a/working_biglist.xlsx
+++ b/working_biglist.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CliffConda\Desktop\Project_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yural\Desktop\Veil_Of_Ignorance\veil_of_ignorance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C71D7E-FC2C-4496-ADC9-21CFB2F34D27}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A507CD3-2D03-44DB-861A-BDAFB1465625}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="table" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="182">
   <si>
     <t>('B15001.  SEX BY AGE BY EDUCATIONAL ATTAINMENT FOR THE POPULATION 18 YEARS AND OVER', "Male:!!18 to 24 years:!!Associate's degree")</t>
   </si>
@@ -358,12 +360,231 @@
   <si>
     <t>Puerto Rico: Summary level: 040, state:72</t>
   </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>some college no degree</t>
+  </si>
+  <si>
+    <t>associates degree</t>
+  </si>
+  <si>
+    <t>bachelors degree</t>
+  </si>
+  <si>
+    <t>graduate or professional degree</t>
+  </si>
+  <si>
+    <t>18-24</t>
+  </si>
+  <si>
+    <t>25-34</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>45-64</t>
+  </si>
+  <si>
+    <t>65  and over</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>some_college_no_degree</t>
+  </si>
+  <si>
+    <t>associates_degree</t>
+  </si>
+  <si>
+    <t>bachelors_degree</t>
+  </si>
+  <si>
+    <t>graduate_or_professional_degree</t>
+  </si>
+  <si>
+    <t>18_to_24</t>
+  </si>
+  <si>
+    <t>25_to_34</t>
+  </si>
+  <si>
+    <t>35_to_44</t>
+  </si>
+  <si>
+    <t>45_to_64</t>
+  </si>
+  <si>
+    <t>65_and_over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +596,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,7 +622,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -417,11 +645,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDCDCDC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDCDCDC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDCDCDC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDCDCDC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDCDCDC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDCDCDC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -430,10 +684,16 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,16 +1031,2632 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A96F7CF-20F3-4A25-894E-7C50FFA64ED4}">
+  <dimension ref="A1:L53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="8.88671875" style="5"/>
+    <col min="4" max="4" width="22.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="5"/>
+    <col min="10" max="10" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="5"/>
+    <col min="12" max="12" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="5">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>40</v>
+      </c>
+      <c r="C2" s="5">
+        <f t="shared" ref="C2:L17" ca="1" si="0">RANDBETWEEN(1,100)</f>
+        <v>72</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="I2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="J2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="L2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5">
+        <f t="shared" ref="B3:L34" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>38</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="C32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="I34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="5">
+        <f t="shared" ref="B35:L53" ca="1" si="2">RANDBETWEEN(1,100)</f>
+        <v>33</v>
+      </c>
+      <c r="C35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="L35" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="C36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="G36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="I36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="C37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="C38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="H38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="I38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="L38" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="C39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="L39" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="C40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="D40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="G40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="I40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="L40" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="C41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="I41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="L41" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="C42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="H42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="I42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="L42" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="C43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="F43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="G43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="I43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="L43" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="C44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="G44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="I44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="J44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="L44" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="C45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="D45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="G45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="I45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="L45" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="C46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="F46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="G46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="J46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="L46" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="C47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="E47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="F47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="G47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="H47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="I47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="J47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="L47" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="C48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="D48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="F48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="G48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="H48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="I48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="J48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="K48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="L48" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="C49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="F49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="G49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="I49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="J49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="K49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="L49" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="C50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="E50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="H50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="J50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="L50" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="G51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="I51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="J51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="L51" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="C52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="D52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="I52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="J52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="K52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="L52" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="C53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="D53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="F53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="G53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="I53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="J53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="L53" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CRA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.77734375" customWidth="1"/>
+    <col min="3" max="3" width="124.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3392,7 +6268,7 @@
       <c r="CQZ1" s="1"/>
       <c r="CRA1" s="1"/>
     </row>
-    <row r="2" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -3568,180 +6444,180 @@
         <v>32332</v>
       </c>
     </row>
-    <row r="3" spans="1:2497" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2497" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>1501</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>1806</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>73</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>18930</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3">
         <v>4936</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3">
         <v>9721</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>2800</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3">
         <v>13119</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3">
         <v>3611</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3">
         <v>7787</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3">
         <v>4589</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3">
         <v>28324</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3">
         <v>7855</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3">
         <v>15901</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3">
         <v>10347</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3">
         <v>8185</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3">
         <v>1545</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3">
         <v>5313</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3">
         <v>4649</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3">
         <v>12757</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3">
         <v>1417</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3">
         <v>2805</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3">
         <v>115</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Y3">
         <v>16676</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="Z3">
         <v>4496</v>
       </c>
-      <c r="AA3" s="5">
+      <c r="AA3">
         <v>12630</v>
       </c>
-      <c r="AB3" s="5">
+      <c r="AB3">
         <v>4171</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AC3">
         <v>12075</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AD3">
         <v>4371</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AE3">
         <v>9797</v>
       </c>
-      <c r="AF3" s="5">
+      <c r="AF3">
         <v>5498</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AG3">
         <v>25359</v>
       </c>
-      <c r="AH3" s="5">
+      <c r="AH3">
         <v>9064</v>
       </c>
-      <c r="AI3" s="5">
+      <c r="AI3">
         <v>16983</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AJ3">
         <v>11027</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AK3">
         <v>8315</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AL3">
         <v>1841</v>
       </c>
-      <c r="AM3" s="5">
+      <c r="AM3">
         <v>5069</v>
       </c>
-      <c r="AN3" s="5">
+      <c r="AN3">
         <v>3639</v>
       </c>
-      <c r="AO3" s="5">
+      <c r="AO3">
         <v>50723</v>
       </c>
-      <c r="AQ3" s="5">
+      <c r="AQ3">
         <v>38722</v>
       </c>
-      <c r="AR3" s="5">
+      <c r="AR3">
         <v>14996</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AS3">
         <v>4541</v>
       </c>
-      <c r="AT3" s="5">
+      <c r="AT3">
         <v>2848</v>
       </c>
-      <c r="AU3" s="5">
+      <c r="AU3">
         <v>45407</v>
       </c>
-      <c r="AV3" s="5">
+      <c r="AV3">
         <v>19772</v>
       </c>
-      <c r="AW3" s="5">
+      <c r="AW3">
         <v>44479</v>
       </c>
-      <c r="AX3" s="5">
+      <c r="AX3">
         <v>18451</v>
       </c>
-      <c r="AY3" s="5">
+      <c r="AY3">
         <v>3730</v>
       </c>
-      <c r="AZ3" s="5">
+      <c r="AZ3">
         <v>2154</v>
       </c>
-      <c r="BA3" s="5">
+      <c r="BA3">
         <v>96130</v>
       </c>
-      <c r="BB3" s="5">
+      <c r="BB3">
         <v>37719</v>
       </c>
-      <c r="BC3" s="5">
+      <c r="BC3">
         <v>83201</v>
       </c>
-      <c r="BD3" s="5">
+      <c r="BD3">
         <v>33447</v>
       </c>
-      <c r="BE3" s="5">
+      <c r="BE3">
         <v>8271</v>
       </c>
-      <c r="BF3" s="5">
+      <c r="BF3">
         <v>5002</v>
       </c>
     </row>
-    <row r="4" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -3917,7 +6793,7 @@
         <v>51274</v>
       </c>
     </row>
-    <row r="5" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -4093,7 +6969,7 @@
         <v>18348</v>
       </c>
     </row>
-    <row r="6" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
@@ -4269,7 +7145,7 @@
         <v>387793</v>
       </c>
     </row>
-    <row r="7" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -4445,7 +7321,7 @@
         <v>57051</v>
       </c>
     </row>
-    <row r="8" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
@@ -4621,7 +7497,7 @@
         <v>40484</v>
       </c>
     </row>
-    <row r="9" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
@@ -4797,7 +7673,7 @@
         <v>10467</v>
       </c>
     </row>
-    <row r="10" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -4973,7 +7849,7 @@
         <v>18221</v>
       </c>
     </row>
-    <row r="11" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
@@ -5149,7 +8025,7 @@
         <v>154629</v>
       </c>
     </row>
-    <row r="12" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -5325,7 +8201,7 @@
         <v>78709</v>
       </c>
     </row>
-    <row r="13" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -5501,7 +8377,7 @@
         <v>12805</v>
       </c>
     </row>
-    <row r="14" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -5677,7 +8553,7 @@
         <v>10653</v>
       </c>
     </row>
-    <row r="15" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
@@ -5853,7 +8729,7 @@
         <v>104191</v>
       </c>
     </row>
-    <row r="16" spans="1:2497" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2497" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
@@ -6029,7 +8905,7 @@
         <v>43040</v>
       </c>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -6205,7 +9081,7 @@
         <v>22403</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
@@ -6381,7 +9257,7 @@
         <v>21879</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
@@ -6557,7 +9433,7 @@
         <v>27802</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
@@ -6733,7 +9609,7 @@
         <v>27903</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -6909,7 +9785,7 @@
         <v>12033</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>77</v>
       </c>
@@ -7085,7 +9961,7 @@
         <v>100946</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -7261,7 +10137,7 @@
         <v>115466</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
@@ -7437,7 +10313,7 @@
         <v>73679</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -7613,7 +10489,7 @@
         <v>47323</v>
       </c>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -7789,7 +10665,7 @@
         <v>17753</v>
       </c>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
@@ -7965,7 +10841,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>83</v>
       </c>
@@ -8141,7 +11017,7 @@
         <v>8546</v>
       </c>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -8317,7 +11193,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>85</v>
       </c>
@@ -8493,7 +11369,7 @@
         <v>16273</v>
       </c>
     </row>
-    <row r="31" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
@@ -8666,7 +11542,7 @@
         <v>13755</v>
       </c>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
@@ -8839,7 +11715,7 @@
         <v>90732</v>
       </c>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>88</v>
       </c>
@@ -9015,7 +11891,7 @@
         <v>25255</v>
       </c>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
@@ -9191,7 +12067,7 @@
         <v>193097</v>
       </c>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>90</v>
       </c>
@@ -9367,7 +12243,7 @@
         <v>84345</v>
       </c>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
@@ -9543,7 +12419,7 @@
         <v>5350</v>
       </c>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>92</v>
       </c>
@@ -9719,7 +12595,7 @@
         <v>82753</v>
       </c>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
@@ -9895,7 +12771,7 @@
         <v>23949</v>
       </c>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
@@ -10071,7 +12947,7 @@
         <v>38791</v>
       </c>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -10247,7 +13123,7 @@
         <v>119014</v>
       </c>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>96</v>
       </c>
@@ -10423,7 +13299,7 @@
         <v>12040</v>
       </c>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>97</v>
       </c>
@@ -10599,7 +13475,7 @@
         <v>32717</v>
       </c>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
@@ -10775,7 +13651,7 @@
         <v>6126</v>
       </c>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
@@ -10951,7 +13827,7 @@
         <v>51579</v>
       </c>
     </row>
-    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>100</v>
       </c>
@@ -11127,7 +14003,7 @@
         <v>177921</v>
       </c>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>101</v>
       </c>
@@ -11303,7 +14179,7 @@
         <v>23017</v>
       </c>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
@@ -11479,7 +14355,7 @@
         <v>7807</v>
       </c>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>103</v>
       </c>
@@ -11655,7 +14531,7 @@
         <v>94853</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>104</v>
       </c>
@@ -11831,7 +14707,7 @@
         <v>67176</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
@@ -12007,7 +14883,7 @@
         <v>10459</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>106</v>
       </c>
@@ -12183,7 +15059,7 @@
         <v>41387</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
@@ -12359,7 +15235,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>108</v>
       </c>
@@ -12533,306 +15409,6 @@
       </c>
       <c r="BF53">
         <v>22364</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A94258-14FB-48C0-BA77-7524652B11ED}">
-  <dimension ref="E6:E62"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E62"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E51" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E55" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E57" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E61" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -12841,6 +15417,347 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A94258-14FB-48C0-BA77-7524652B11ED}">
+  <dimension ref="A2:O62"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="173.44140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E32" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E43" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E53" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E55" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E56" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E57" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E59" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E60" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E61" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E62" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881F6DB8-5C53-4BF4-8D9A-38E976FCDABB}">
   <dimension ref="A1:BF53"/>
   <sheetViews>
@@ -12848,9 +15765,9 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13023,7 +15940,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -13256,7 +16173,7 @@
         <v>32332</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -13489,7 +16406,7 @@
         <v>5002</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -13722,7 +16639,7 @@
         <v>51274</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -13955,7 +16872,7 @@
         <v>18348</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
@@ -14188,7 +17105,7 @@
         <v>387793</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -14421,7 +17338,7 @@
         <v>57051</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
@@ -14654,7 +17571,7 @@
         <v>40484</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
@@ -14887,7 +17804,7 @@
         <v>10467</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -15120,7 +18037,7 @@
         <v>18221</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
@@ -15353,7 +18270,7 @@
         <v>154629</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -15586,7 +18503,7 @@
         <v>78709</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -15819,7 +18736,7 @@
         <v>12805</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -16052,7 +18969,7 @@
         <v>10653</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
@@ -16285,7 +19202,7 @@
         <v>104191</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
@@ -16518,7 +19435,7 @@
         <v>43040</v>
       </c>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -16751,7 +19668,7 @@
         <v>22403</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
@@ -16984,7 +19901,7 @@
         <v>21879</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
@@ -17217,7 +20134,7 @@
         <v>27802</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
@@ -17450,7 +20367,7 @@
         <v>27903</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -17683,7 +20600,7 @@
         <v>12033</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>77</v>
       </c>
@@ -17916,7 +20833,7 @@
         <v>100946</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -18149,7 +21066,7 @@
         <v>115466</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
@@ -18382,7 +21299,7 @@
         <v>73679</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -18615,7 +21532,7 @@
         <v>47323</v>
       </c>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -18848,7 +21765,7 @@
         <v>17753</v>
       </c>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
@@ -19081,7 +21998,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>83</v>
       </c>
@@ -19314,7 +22231,7 @@
         <v>8546</v>
       </c>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -19547,7 +22464,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>85</v>
       </c>
@@ -19780,7 +22697,7 @@
         <v>16273</v>
       </c>
     </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
@@ -20013,7 +22930,7 @@
         <v>13755</v>
       </c>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
@@ -20246,7 +23163,7 @@
         <v>90732</v>
       </c>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>88</v>
       </c>
@@ -20479,7 +23396,7 @@
         <v>25255</v>
       </c>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
@@ -20712,7 +23629,7 @@
         <v>193097</v>
       </c>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>90</v>
       </c>
@@ -20945,7 +23862,7 @@
         <v>84345</v>
       </c>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
@@ -21178,7 +24095,7 @@
         <v>5350</v>
       </c>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>92</v>
       </c>
@@ -21411,7 +24328,7 @@
         <v>82753</v>
       </c>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
@@ -21644,7 +24561,7 @@
         <v>23949</v>
       </c>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
@@ -21877,7 +24794,7 @@
         <v>38791</v>
       </c>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -22110,7 +25027,7 @@
         <v>119014</v>
       </c>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>96</v>
       </c>
@@ -22343,7 +25260,7 @@
         <v>12040</v>
       </c>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>97</v>
       </c>
@@ -22576,7 +25493,7 @@
         <v>32717</v>
       </c>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
@@ -22809,7 +25726,7 @@
         <v>6126</v>
       </c>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
@@ -23042,7 +25959,7 @@
         <v>51579</v>
       </c>
     </row>
-    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>100</v>
       </c>
@@ -23275,7 +26192,7 @@
         <v>177921</v>
       </c>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>101</v>
       </c>
@@ -23508,7 +26425,7 @@
         <v>23017</v>
       </c>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
@@ -23741,7 +26658,7 @@
         <v>7807</v>
       </c>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>103</v>
       </c>
@@ -23974,7 +26891,7 @@
         <v>94853</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>104</v>
       </c>
@@ -24207,7 +27124,7 @@
         <v>67176</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
@@ -24440,19 +27357,89 @@
         <v>10459</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D9E3A1-E4A8-4B45-A9C6-CDA7F8661108}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>